<commit_message>
[vignettes] Update iris scale info
Column names have changed.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_iris_scaleInfo.xlsx
+++ b/inst/extdata/example_iris_scaleInfo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">varName</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t xml:space="preserve">Items_der_Skala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imputationen</t>
   </si>
 </sst>
 </file>
@@ -368,6 +371,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>